<commit_message>
adjusted column names in the spreadsheet
</commit_message>
<xml_diff>
--- a/TestStatementsSheet.xlsx
+++ b/TestStatementsSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\Desktop\Projects\email-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40D081DA-3BF4-4F44-A557-621D2474880B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0503E2-22E3-4B79-9108-EC310A2345C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23010" yWindow="7970" windowWidth="7500" windowHeight="6000" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Attachment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>David</t>
   </si>
@@ -67,6 +58,30 @@
   </si>
   <si>
     <t>C:\Users\adavi\OneDrive\Documents\Attachment C.pdf</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>filepath</t>
+  </si>
+  <si>
+    <t>123 Fake St, Fake</t>
   </si>
 </sst>
 </file>
@@ -438,79 +453,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC3CB26-7A67-44E4-BD6D-0ABC7E302C80}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.08984375" customWidth="1"/>
     <col min="2" max="2" width="27.36328125" customWidth="1"/>
-    <col min="3" max="3" width="112.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="112.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
renamed filename column to filenames in spreadsheet
</commit_message>
<xml_diff>
--- a/TestStatementsSheet.xlsx
+++ b/TestStatementsSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\Desktop\Projects\email-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0503E2-22E3-4B79-9108-EC310A2345C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A25FF4-CB61-4726-BEDF-DF94E43EBE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
+    <workbookView xWindow="13770" yWindow="5450" windowWidth="7500" windowHeight="6000" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Citizen</t>
   </si>
   <si>
-    <t>C:\Users\adavi\OneDrive\Documents\Attachment A.pdf</t>
-  </si>
-  <si>
     <t>C:\Users\adavi\OneDrive\Documents\Attachment B.pdf</t>
   </si>
   <si>
@@ -78,10 +75,13 @@
     <t>property</t>
   </si>
   <si>
-    <t>filepath</t>
-  </si>
-  <si>
     <t>123 Fake St, Fake</t>
+  </si>
+  <si>
+    <t>C:\Users\adavi\OneDrive\Documents\Attachment A.pdf;C:\Users\adavi\OneDrive\Documents\Attachment B.pdf</t>
+  </si>
+  <si>
+    <t>filepaths</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC3CB26-7A67-44E4-BD6D-0ABC7E302C80}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,16 +469,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -489,10 +489,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -503,10 +503,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -517,10 +517,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -531,10 +531,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added send email call
</commit_message>
<xml_diff>
--- a/TestStatementsSheet.xlsx
+++ b/TestStatementsSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\Desktop\Projects\email-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A25FF4-CB61-4726-BEDF-DF94E43EBE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D350AE-9E85-40EF-8E5C-C426ACE50990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="5450" windowWidth="7500" windowHeight="6000" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,15 +455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC3CB26-7A67-44E4-BD6D-0ABC7E302C80}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.08984375" customWidth="1"/>
     <col min="2" max="2" width="27.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="66.81640625" customWidth="1"/>
     <col min="4" max="4" width="112.1796875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added subject field to the spreadsheet
</commit_message>
<xml_diff>
--- a/TestStatementsSheet.xlsx
+++ b/TestStatementsSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\Desktop\Projects\email-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D350AE-9E85-40EF-8E5C-C426ACE50990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7BEBE2-3702-4AE2-BED0-81A927DA7961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{747F1B62-10B8-4964-977E-C2D823A1186C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>David</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>filepaths</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC3CB26-7A67-44E4-BD6D-0ABC7E302C80}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,9 +468,10 @@
     <col min="2" max="2" width="27.36328125" customWidth="1"/>
     <col min="3" max="3" width="66.81640625" customWidth="1"/>
     <col min="4" max="4" width="112.1796875" customWidth="1"/>
+    <col min="5" max="5" width="25.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -480,8 +484,11 @@
       <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -494,8 +501,12 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="str">
+        <f>_xlfn.CONCAT(C2, " - Owner Statement")</f>
+        <v>123 Fake St, Fake - Owner Statement</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -508,8 +519,12 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="str">
+        <f>_xlfn.CONCAT(C3, " - Owner Statement")</f>
+        <v>B - Owner Statement</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -522,8 +537,12 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="str">
+        <f>_xlfn.CONCAT(C4, " - Owner Statement")</f>
+        <v>C - Owner Statement</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -536,12 +555,16 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" t="str">
+        <f>_xlfn.CONCAT(C5, " - Owner Statement")</f>
+        <v>D - Owner Statement</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>

</xml_diff>